<commit_message>
Liste des tâches part II
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0636FB5D-4242-470C-986A-469A9F09775F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21985A9A-8621-4620-B773-492CC5A8EF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Tâches</t>
   </si>
@@ -54,6 +54,57 @@
   </si>
   <si>
     <t>CRUD pour les employees</t>
+  </si>
+  <si>
+    <t>CRUD Rendez-vous</t>
+  </si>
+  <si>
+    <t>Écrire les rapports</t>
+  </si>
+  <si>
+    <t>Consulter les dossier des animaux</t>
+  </si>
+  <si>
+    <t>VÉTÉRINAIRE</t>
+  </si>
+  <si>
+    <t>SECRÉTAIRE</t>
+  </si>
+  <si>
+    <t>CRUD des animaux</t>
+  </si>
+  <si>
+    <t>CRUD des propriétaire</t>
+  </si>
+  <si>
+    <t>Accueil "HistoryVisit"</t>
+  </si>
+  <si>
+    <t>Accueil. Consulter les rendez-vous</t>
+  </si>
+  <si>
+    <t>Accueil "VisitsForToday" ou "ActiveVisitsForPets"</t>
+  </si>
+  <si>
+    <t>Voir les disponibilités des vétérinaires</t>
+  </si>
+  <si>
+    <t>Gérer les disponibilités</t>
+  </si>
+  <si>
+    <t>Voir l'horaire au complet "VeterinarySchedule"</t>
+  </si>
+  <si>
+    <t>PAGE RENDEZ-VOUS</t>
+  </si>
+  <si>
+    <t>Accueil "OnGoingVisits"</t>
+  </si>
+  <si>
+    <t>Dans la page de l'animal, ajoute la view "ActivePetTreatments"</t>
+  </si>
+  <si>
+    <t>Dans la page pour gérer les employees, l'accueil "EmployeeContacts"</t>
   </si>
 </sst>
 </file>
@@ -97,9 +148,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91C581-3801-4311-8797-DBD170BF6C7C}">
-  <dimension ref="A2:C5"/>
+  <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -468,8 +531,99 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Page Login et connection avec la database done.
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21985A9A-8621-4620-B773-492CC5A8EF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E412D-2210-4443-8CF3-26B384C8171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Tâches</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Accueil "HistoryVisit"</t>
   </si>
   <si>
-    <t>Accueil. Consulter les rendez-vous</t>
-  </si>
-  <si>
     <t>Accueil "VisitsForToday" ou "ActiveVisitsForPets"</t>
   </si>
   <si>
@@ -105,6 +102,15 @@
   </si>
   <si>
     <t>Dans la page pour gérer les employees, l'accueil "EmployeeContacts"</t>
+  </si>
+  <si>
+    <t>Alejandro</t>
+  </si>
+  <si>
+    <t>Accueil. Consulter les rendez-vous "VisitsForToday"</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
@@ -148,13 +154,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -167,7 +170,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -500,7 +525,7 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +549,12 @@
       <c r="A3" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -536,8 +567,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
+      <c r="A6" s="4" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -547,7 +578,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,12 +591,12 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -579,13 +610,13 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>21</v>
+      <c r="A16" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
@@ -594,8 +625,8 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>15</v>
+      <c r="A20" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -612,8 +643,8 @@
       <c r="A23" s="2"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>19</v>
+      <c r="A24" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
@@ -623,10 +654,18 @@
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"YES"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Page d'accueil pour les veterinaires done (Juste le view et le design, il manque les btn)
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E412D-2210-4443-8CF3-26B384C8171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A96F77-D277-4EE0-BD50-CCF14F3CA211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Tâches</t>
   </si>
@@ -170,7 +170,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -182,13 +182,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -525,7 +518,7 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +591,12 @@
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -659,11 +658,11 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"YES"</formula>
-    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NO"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"YES"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Design of the Admin Form + Visit History functionality with filtering options.
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269E412D-2210-4443-8CF3-26B384C8171A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF1C63B-BD40-4262-BDA7-61E788E0D994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -117,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,14 +168,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -525,16 +516,16 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +536,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -556,113 +547,113 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ajout de current assigned task in the exel file.
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A96F77-D277-4EE0-BD50-CCF14F3CA211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213A2BB-A12D-4085-9C97-F87248B83258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
+    <workbookView xWindow="30612" yWindow="-4056" windowWidth="13176" windowHeight="23256" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
   <si>
     <t>Tâches</t>
   </si>
@@ -111,13 +109,22 @@
   </si>
   <si>
     <t>YES</t>
+  </si>
+  <si>
+    <t>Gino</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gino </t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,16 +525,16 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.09765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -549,45 +556,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -598,60 +629,60 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Creation du webformPet pour gestion des Pets
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\source\repos\AnimalCare_dbFirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fosso frank\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E213A2BB-A12D-4085-9C97-F87248B83258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74535C8F-3818-43A5-82E9-AEB1FB20E334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-4056" windowWidth="13176" windowHeight="23256" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Tâches</t>
   </si>
@@ -118,13 +118,16 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>Fosso</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,17 +527,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91C581-3801-4311-8797-DBD170BF6C7C}">
   <dimension ref="A2:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="65.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -556,12 +559,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -572,7 +575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -583,7 +586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -594,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -605,20 +608,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -629,60 +632,69 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="21" spans="1:1">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:1">
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Ajoute des variables de session dans la page de login, admin, vet et rec
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeann\source\repos\AnimalCare_dbFirst\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{031C39E7-4C77-40D5-9FE1-9BB82EEEBE61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AE30E1-7BDD-46CA-88F7-2AC20C37BEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-4056" windowWidth="13176" windowHeight="23256" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Tâches</t>
   </si>
@@ -127,7 +127,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -528,16 +528,16 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="65.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +548,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -559,12 +559,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
@@ -586,7 +586,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -597,7 +597,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -608,20 +608,20 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -632,22 +632,22 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -658,12 +658,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>14</v>
       </c>
@@ -674,35 +674,44 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
       <c r="C21" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="B25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="B26" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Création WebFormVisit(Juste le designe
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8AE30E1-7BDD-46CA-88F7-2AC20C37BEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1303B1-BD4F-4985-953D-B34F0DA07E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
   <si>
     <t>Tâches</t>
   </si>
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF91C581-3801-4311-8797-DBD170BF6C7C}">
   <dimension ref="A2:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>28</v>
       </c>
       <c r="C20" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>28</v>
       </c>
       <c r="C21" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -705,6 +705,9 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
+      <c r="C25" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
@@ -712,6 +715,9 @@
       </c>
       <c r="B26" t="s">
         <v>22</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mise à jour l'excel
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1303B1-BD4F-4985-953D-B34F0DA07E88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D849C5C3-7C8A-49C9-9D1D-2DB6CAFA9B7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,7 +717,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WebForm visit done avec tout les btn
</commit_message>
<xml_diff>
--- a/Taches.xlsx
+++ b/Taches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejo\source\repos\AnimalCare_dbFirst\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ECB0D8-15DC-4E19-A212-2CFC8F5615FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D1F455-B58E-4350-A609-306D84929572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2F3325C4-01DA-4B1F-8C6D-B15FBC8CD45B}"/>
   </bookViews>
@@ -93,9 +93,6 @@
     <t>PAGE RENDEZ-VOUS</t>
   </si>
   <si>
-    <t>Accueil "OnGoingVisits"</t>
-  </si>
-  <si>
     <t>Dans la page de l'animal, ajoute la view "ActivePetTreatments"</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Fosso</t>
+  </si>
+  <si>
+    <t>Accueil "ActiveVisitsForPets" et "VeterinaryAvailabilityForWeek"</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A2:C26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,10 +553,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -569,21 +569,21 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -591,10 +591,10 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -602,10 +602,10 @@
         <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,13 +623,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
         <v>23</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,10 +652,10 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -668,10 +668,10 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -679,10 +679,10 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -703,21 +703,21 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>